<commit_message>
fix: fixed typescript issue
</commit_message>
<xml_diff>
--- a/public/sample-files/sample_payments.xlsx
+++ b/public/sample-files/sample_payments.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Employee</t>
   </si>
   <si>
-    <t xml:space="preserve">Paid</t>
+    <t xml:space="preserve">Paisd</t>
   </si>
   <si>
     <t xml:space="preserve">Alice</t>
@@ -168,7 +168,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>